<commit_message>
Updated Manuscript and Supplementary Materials
</commit_message>
<xml_diff>
--- a/experiment 0/data/raw/codebook_raw_data.xlsx
+++ b/experiment 0/data/raw/codebook_raw_data.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamiecummins/git/amp-intentionality/experiment 2/data/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean\Desktop\git\amp-awareness\experiment 0\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8B7E3F-5B17-D147-BB30-3C7339202E7B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15780" yWindow="2040" windowWidth="30260" windowHeight="17540" tabRatio="583" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15780" yWindow="2040" windowWidth="30264" windowHeight="17544" tabRatio="583" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="modified_intentionality_amp" sheetId="14" r:id="rId1"/>
-    <sheet name="demographics" sheetId="13" r:id="rId2"/>
-    <sheet name="post_questions" sheetId="15" r:id="rId3"/>
-    <sheet name="standard_amp" sheetId="16" r:id="rId4"/>
+    <sheet name="demographics" sheetId="13" r:id="rId1"/>
+    <sheet name="skip_amp" sheetId="14" r:id="rId2"/>
+    <sheet name="standard_amp" sheetId="16" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000"/>
   <extLst>
@@ -28,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
   <si>
     <t>variable</t>
   </si>
@@ -57,12 +55,6 @@
     <t>subject identifier</t>
   </si>
   <si>
-    <t>build</t>
-  </si>
-  <si>
-    <t>version of Inquisit experiment was run in</t>
-  </si>
-  <si>
     <t>blocknum</t>
   </si>
   <si>
@@ -87,27 +79,9 @@
     <t>name of current trial</t>
   </si>
   <si>
-    <t>pretrialpause</t>
-  </si>
-  <si>
     <t>unused variable</t>
   </si>
   <si>
-    <t>posttrialpause</t>
-  </si>
-  <si>
-    <t>windowcenter</t>
-  </si>
-  <si>
-    <t>trialduration</t>
-  </si>
-  <si>
-    <t>trialtimeout</t>
-  </si>
-  <si>
-    <t>blocktimeout</t>
-  </si>
-  <si>
     <t>response</t>
   </si>
   <si>
@@ -120,12 +94,6 @@
     <t>latency</t>
   </si>
   <si>
-    <t>time taken to provide response</t>
-  </si>
-  <si>
-    <t>inwindow</t>
-  </si>
-  <si>
     <t>name of current trial (if trialcode begins with "prime", then this identifies the prime stimulus presented during an AMP trial; if trialcode begins with "intention", then this refers to the influence-awareness check)</t>
   </si>
   <si>
@@ -159,20 +127,20 @@
     <t>the total cumulative percent of trials with negative prime stimuli where the participant responded with pleasant</t>
   </si>
   <si>
-    <t>name of current block; if blockcode ends in "ufirst", then the unintentionality self-report question was presented before the intentionality self-report question. The opposite was the case for blockcodes ending in "ifirst".</t>
-  </si>
-  <si>
     <t>name of current trial (identifies if prime was positive or negative)</t>
   </si>
   <si>
     <t xml:space="preserve">If correct == 0, then the participant rated the target as unpleasant, and if correct == 1, then the participant rated the target as pleasant. </t>
+  </si>
+  <si>
+    <t>response emitted by the participant</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -211,19 +179,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1104,15 +1060,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1131,32 +1084,32 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="783">
@@ -2278,20 +2231,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A9" sqref="A9:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.796875" customWidth="1"/>
     <col min="2" max="2" width="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2299,112 +2252,69 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="11"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="11"/>
-    </row>
-    <row r="7" spans="1:3" ht="36" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="11"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="24" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="24" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>42</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2418,20 +2328,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B20" sqref="A1:B20"/>
+      <selection activeCell="A12" sqref="A12:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.796875" customWidth="1"/>
     <col min="2" max="2" width="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2439,167 +2349,88 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:3" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="10"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="11"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="11"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="B10" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="B11" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2613,207 +2444,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C20"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.83203125" customWidth="1"/>
-    <col min="2" max="2" width="55" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="11"/>
-    </row>
-    <row r="7" spans="1:3" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="11"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D8C1D9-3589-5445-8AB2-7B8133428F99}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.796875" customWidth="1"/>
     <col min="2" max="2" width="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2821,111 +2465,111 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="11"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="B7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="11"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="11"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="16" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="24" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
+    </row>
+    <row r="13" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="24" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="24" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>42</v>
+      <c r="B13" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>